<commit_message>
PROS-9204 - MARSRU - New KPI Set
</commit_message>
<xml_diff>
--- a/Projects/MARSRU2_SAND/Data/2018/MARS KPIs.xlsx
+++ b/Projects/MARSRU2_SAND/Data/2018/MARS KPIs.xlsx
@@ -29,9 +29,9 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
@@ -46,6 +46,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -116,7 +117,7 @@
     <t xml:space="preserve">Manufacturer</t>
   </si>
   <si>
-    <t xml:space="preserve">Brand Category value</t>
+    <t xml:space="preserve">Category</t>
   </si>
   <si>
     <t xml:space="preserve">Sub brand to include</t>
@@ -1602,35 +1603,35 @@
   </sheetPr>
   <dimension ref="1:72"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.7408906882591"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="2" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="3" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="99.2995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="102.728744939271"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="100.263157894737"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="103.692307692308"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="38.2429149797571"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="3" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="2" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="2" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="3" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="4" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="4" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="22" min="19" style="3" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="3" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="3" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="4" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="3" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="3" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="4" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="29" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -65718,13 +65719,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -65750,10 +65751,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="37.2793522267206"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="25" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="25" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="26" width="11.0323886639676"/>
   </cols>
   <sheetData>
@@ -65852,10 +65853,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="37.2793522267206"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="26" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="26" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="26" width="11.0323886639676"/>
   </cols>
   <sheetData>
@@ -65953,10 +65954,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.3441295546559"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.8785425101215"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -66082,10 +66083,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="33" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="66.6275303643725"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="67.2712550607288"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="36.5263157894737"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="33" width="11.0323886639676"/>
   </cols>
   <sheetData>
@@ -66211,8 +66212,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="54.9514170040486"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="55.4858299595142"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="25" width="10.7125506072875"/>
   </cols>
   <sheetData>
@@ -66320,14 +66321,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -68801,10 +68802,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -68851,8 +68852,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="36" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>